<commit_message>
Update new username and password
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/testData/loginData.xlsx
+++ b/src/test/java/com/inetbanking/testData/loginData.xlsx
@@ -1,34 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9BEF8B29-FBE9-4B09-A280-968484D22C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\eclipse-workspace\inetBanking\src\test\java\com\inetbanking\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4BA785-320E-43F3-910F-2066A2DC0CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BBD4A10-E3A8-49CF-8781-2F2B90D1E783}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -36,10 +33,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>mngr502803</t>
+    <t>mngr515202</t>
   </si>
   <si>
-    <t>EgUgumy</t>
+    <t>usYrumy</t>
   </si>
 </sst>
 </file>
@@ -111,7 +108,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -123,7 +120,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -170,23 +167,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -222,23 +202,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -390,8 +353,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57016226-77B3-4180-9EFF-C5840AFBB019}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -423,14 +386,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>